<commit_message>
European colonial range penalty now scales with tech
And is generally much less severe, while still preventing reaching the Americas
-Europeans and Muslims now cannot pick exploration ideas until Colonialism is enabled
-Portugal now starts with the ability to recruit Explorers and Conquistadors, colonial range bonus was moved to the first idea
</commit_message>
<xml_diff>
--- a/.archive/spreadsheets/range_calc.xlsx
+++ b/.archive/spreadsheets/range_calc.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Uros\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Uros\Documents\Paradox Interactive\Europa Universalis IV\mod\third_odyssey_DEV\.archive\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B67D994F-5BBE-477D-B156-6F3C042BD586}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DACADEB8-3D9E-472F-869A-30E3965C3F1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2E20644D-2D29-4DA8-83C9-CAA202C95173}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>Base range</t>
   </si>
@@ -62,6 +62,12 @@
   </si>
   <si>
     <t>Range +50%</t>
+  </si>
+  <si>
+    <t>MIN</t>
+  </si>
+  <si>
+    <t>MAX</t>
   </si>
 </sst>
 </file>
@@ -414,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA765C9F-47F0-405C-8CEF-CDD236D5CD8D}">
-  <dimension ref="B2:L10"/>
+  <dimension ref="A2:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -426,7 +432,7 @@
     <col min="11" max="11" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -437,7 +443,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B3">
         <f>IF(C3&gt;=7,IF(C3&gt;=9,325,275),160)</f>
         <v>275</v>
@@ -465,7 +471,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H4">
         <v>0.5</v>
       </c>
@@ -476,7 +482,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K5" t="s">
         <v>6</v>
       </c>
@@ -484,7 +490,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E6" t="s">
         <v>3</v>
       </c>
@@ -495,7 +501,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E7">
         <f>B3*(1+E3)</f>
         <v>151.25</v>
@@ -507,15 +513,201 @@
         <v>164</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E10">
         <f>B3*1.5</f>
         <v>412.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H14">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15">
+        <v>150</v>
+      </c>
+      <c r="C15">
+        <v>160</v>
+      </c>
+      <c r="D15">
+        <v>0.05</v>
+      </c>
+      <c r="E15">
+        <f>C15*(1-D15)</f>
+        <v>152</v>
+      </c>
+      <c r="G15">
+        <v>0.05</v>
+      </c>
+      <c r="H15">
+        <f>C15*(1-G15+$H$14)</f>
+        <v>192</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16">
+        <v>231</v>
+      </c>
+      <c r="C16">
+        <v>275</v>
+      </c>
+      <c r="D16">
+        <v>0.4</v>
+      </c>
+      <c r="E16">
+        <f t="shared" ref="E16:E18" si="0">C16*(1-D16)</f>
+        <v>165</v>
+      </c>
+      <c r="G16">
+        <v>0.5</v>
+      </c>
+      <c r="H16">
+        <f t="shared" ref="H16:H18" si="1">C16*(1-G16+$H$14)</f>
+        <v>206.25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <v>325</v>
+      </c>
+      <c r="D17">
+        <v>0.45</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>178.75000000000003</v>
+      </c>
+      <c r="G17">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="1"/>
+        <v>227.49999999999997</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C18">
+        <v>425</v>
+      </c>
+      <c r="D18">
+        <v>0.5</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>212.5</v>
+      </c>
+      <c r="G18">
+        <v>0.6</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="1"/>
+        <v>276.25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H21">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22">
+        <v>150</v>
+      </c>
+      <c r="C22">
+        <v>160</v>
+      </c>
+      <c r="D22">
+        <v>0.1</v>
+      </c>
+      <c r="E22">
+        <f>C22*(1-D22)</f>
+        <v>144</v>
+      </c>
+      <c r="G22">
+        <v>0.3</v>
+      </c>
+      <c r="H22">
+        <f>C22*(1-G22+$H$14)</f>
+        <v>152</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23">
+        <v>154</v>
+      </c>
+      <c r="C23">
+        <v>260</v>
+      </c>
+      <c r="D23">
+        <v>0.42</v>
+      </c>
+      <c r="E23">
+        <f t="shared" ref="E23:E25" si="2">C23*(1-D23)</f>
+        <v>150.80000000000001</v>
+      </c>
+      <c r="G23">
+        <v>0.66</v>
+      </c>
+      <c r="H23">
+        <f t="shared" ref="H23:H25" si="3">C23*(1-G23+$H$14)</f>
+        <v>153.4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C24">
+        <v>310</v>
+      </c>
+      <c r="D24">
+        <v>0.51</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="2"/>
+        <v>151.9</v>
+      </c>
+      <c r="G24">
+        <v>0.755</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="3"/>
+        <v>153.44999999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C25">
+        <v>410</v>
+      </c>
+      <c r="D25">
+        <v>0.6</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="2"/>
+        <v>164</v>
+      </c>
+      <c r="G25">
+        <v>0.8</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="3"/>
+        <v>184.49999999999997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed a bug where Portugal was able to colonize new world to early if lied to
</commit_message>
<xml_diff>
--- a/.archive/spreadsheets/range_calc.xlsx
+++ b/.archive/spreadsheets/range_calc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Uros\Documents\Paradox Interactive\Europa Universalis IV\mod\third_odyssey_DEV\.archive\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DACADEB8-3D9E-472F-869A-30E3965C3F1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47DD3135-7851-4A5F-B68C-5A89DB673BEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2E20644D-2D29-4DA8-83C9-CAA202C95173}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2E20644D-2D29-4DA8-83C9-CAA202C95173}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -19,13 +19,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -423,16 +416,16 @@
   <dimension ref="A2:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.42578125" customWidth="1"/>
-    <col min="11" max="11" width="16.140625" customWidth="1"/>
+    <col min="2" max="2" width="11.44140625" customWidth="1"/>
+    <col min="11" max="11" width="16.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -443,7 +436,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B3">
         <f>IF(C3&gt;=7,IF(C3&gt;=9,325,275),160)</f>
         <v>275</v>
@@ -471,7 +464,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="H4">
         <v>0.5</v>
       </c>
@@ -482,7 +475,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="K5" t="s">
         <v>6</v>
       </c>
@@ -490,7 +483,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E6" t="s">
         <v>3</v>
       </c>
@@ -501,7 +494,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E7">
         <f>B3*(1+E3)</f>
         <v>151.25</v>
@@ -513,23 +506,23 @@
         <v>164</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E10">
         <f>B3*1.5</f>
         <v>412.5</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="H14">
         <v>0.25</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -554,7 +547,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -579,7 +572,7 @@
         <v>206.25</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C17">
         <v>325</v>
       </c>
@@ -598,7 +591,7 @@
         <v>227.49999999999997</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C18">
         <v>425</v>
       </c>
@@ -617,97 +610,97 @@
         <v>276.25</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="H21">
         <v>0.25</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>10</v>
       </c>
       <c r="B22">
-        <v>150</v>
+        <v>116</v>
       </c>
       <c r="C22">
         <v>160</v>
       </c>
       <c r="D22">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="E22">
         <f>C22*(1-D22)</f>
-        <v>144</v>
+        <v>112</v>
       </c>
       <c r="G22">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="H22">
         <f>C22*(1-G22+$H$14)</f>
-        <v>152</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>11</v>
       </c>
       <c r="B23">
-        <v>154</v>
+        <v>138</v>
       </c>
       <c r="C23">
         <v>260</v>
       </c>
       <c r="D23">
-        <v>0.42</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="E23">
         <f t="shared" ref="E23:E25" si="2">C23*(1-D23)</f>
-        <v>150.80000000000001</v>
+        <v>116.99999999999999</v>
       </c>
       <c r="G23">
-        <v>0.66</v>
+        <v>0.72499999999999998</v>
       </c>
       <c r="H23">
         <f t="shared" ref="H23:H25" si="3">C23*(1-G23+$H$14)</f>
-        <v>153.4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+        <v>136.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C24">
         <v>310</v>
       </c>
       <c r="D24">
-        <v>0.51</v>
+        <v>0.6</v>
       </c>
       <c r="E24">
         <f t="shared" si="2"/>
-        <v>151.9</v>
+        <v>124</v>
       </c>
       <c r="G24">
-        <v>0.755</v>
+        <v>0.75</v>
       </c>
       <c r="H24">
         <f t="shared" si="3"/>
-        <v>153.44999999999999</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C25">
         <v>410</v>
       </c>
       <c r="D25">
-        <v>0.6</v>
+        <v>0.65</v>
       </c>
       <c r="E25">
         <f t="shared" si="2"/>
-        <v>164</v>
+        <v>143.5</v>
       </c>
       <c r="G25">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
       <c r="H25">
         <f t="shared" si="3"/>
-        <v>184.49999999999997</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Portugal will no longer colonise Americas if you lie to them and they don't have colonialism, this time for real. This won't work if they are already there in an ongoing game.
</commit_message>
<xml_diff>
--- a/.archive/spreadsheets/range_calc.xlsx
+++ b/.archive/spreadsheets/range_calc.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Uros\Documents\Paradox Interactive\Europa Universalis IV\mod\third_odyssey_DEV\.archive\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47DD3135-7851-4A5F-B68C-5A89DB673BEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EB3FD25-A7D6-40DC-946E-7D23F7457D23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2E20644D-2D29-4DA8-83C9-CAA202C95173}"/>
   </bookViews>
@@ -416,7 +416,7 @@
   <dimension ref="A2:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -677,11 +677,11 @@
         <v>124</v>
       </c>
       <c r="G24">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="H24">
         <f t="shared" si="3"/>
-        <v>155</v>
+        <v>139.5</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>